<commit_message>
added Brent 1997 study
</commit_message>
<xml_diff>
--- a/Studies_from_Zhou_NMA.xlsx
+++ b/Studies_from_Zhou_NMA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcjtrde_ucl_ac_uk/Documents/AIM Lab/Apples and Oranges/Revision 1/Updated Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphaelle\Documents\AIM Lab\apples_and_oranges\main_git\apples_oranges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{335FDCE1-2C2D-42F1-9451-32C5A30EAD2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{52B1DC82-3199-4D47-817B-81700094C625}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0F7C9A9-2C01-46B0-A1A7-CA19B7BD1BDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17560" windowHeight="5810" xr2:uid="{88929F6D-EA7A-425D-B888-A9B6898AEC85}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="65">
   <si>
     <t>Column1</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t>at least one incident of interpersonal trauma (physical, sexual or verbal/emotional abuse)</t>
+  </si>
+  <si>
+    <t>Brent, 1997</t>
+  </si>
+  <si>
+    <t>individual nondirective supportive therapy (NST)</t>
+  </si>
+  <si>
+    <t>systemic behavior family therapy</t>
+  </si>
+  <si>
+    <t>mdd</t>
   </si>
 </sst>
 </file>
@@ -256,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -264,6 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28EF2BE-480A-4658-8587-AC35DFA5CE6A}">
-  <dimension ref="A1:AK5"/>
+  <dimension ref="A1:AK8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="N6" sqref="N6:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1154,12 +1167,253 @@
         <v>1.53</v>
       </c>
     </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>128</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1997</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6">
+        <v>5.7</v>
+      </c>
+      <c r="L6">
+        <v>8.6</v>
+      </c>
+      <c r="M6">
+        <v>35</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P6" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q6">
+        <v>24.3</v>
+      </c>
+      <c r="R6">
+        <v>8.1</v>
+      </c>
+      <c r="S6" s="2">
+        <v>37</v>
+      </c>
+      <c r="T6" s="2">
+        <v>25.7</v>
+      </c>
+      <c r="U6" s="2">
+        <v>7.8</v>
+      </c>
+      <c r="V6" s="2">
+        <v>35</v>
+      </c>
+      <c r="W6" s="2">
+        <v>51.9</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF6">
+        <v>15.7</v>
+      </c>
+      <c r="AG6">
+        <v>1.3</v>
+      </c>
+      <c r="AH6">
+        <v>15.7</v>
+      </c>
+      <c r="AI6">
+        <v>1.5</v>
+      </c>
+      <c r="AJ6">
+        <v>15.6</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>129</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1997</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7">
+        <v>9.1</v>
+      </c>
+      <c r="L7">
+        <v>9.1</v>
+      </c>
+      <c r="M7">
+        <v>29</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q7">
+        <v>22.6</v>
+      </c>
+      <c r="R7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="S7" s="2">
+        <v>35</v>
+      </c>
+      <c r="T7" s="2">
+        <v>25.7</v>
+      </c>
+      <c r="U7" s="2">
+        <v>7.8</v>
+      </c>
+      <c r="V7" s="2">
+        <v>35</v>
+      </c>
+      <c r="W7" s="2">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF7">
+        <v>15.4</v>
+      </c>
+      <c r="AG7">
+        <v>1.4</v>
+      </c>
+      <c r="AH7">
+        <v>15.7</v>
+      </c>
+      <c r="AI7">
+        <v>1.5</v>
+      </c>
+      <c r="AJ7">
+        <v>15.6</v>
+      </c>
+      <c r="AK7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001420048BFE0EA244874208212AE11555" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2670892ea843163c322ab8931abbd97">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0803544b-1b20-413f-a04b-47c23c09c8f3" xmlns:ns4="bdfa4711-3526-46a9-86fc-45ee7e9669d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="953c23f3011a499524bf240fdec3193f" ns3:_="" ns4:_="">
     <xsd:import namespace="0803544b-1b20-413f-a04b-47c23c09c8f3"/>
@@ -1406,15 +1660,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1424,6 +1669,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666C64CD-9023-4136-A743-A40A97E17A25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{370D55A4-0376-4F98-A05F-2BE286C67C7F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1442,27 +1695,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666C64CD-9023-4136-A743-A40A97E17A25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18ECBF79-BB4A-488F-B9C8-31A27F727F35}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="bdfa4711-3526-46a9-86fc-45ee7e9669d1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bdfa4711-3526-46a9-86fc-45ee7e9669d1"/>
     <ds:schemaRef ds:uri="0803544b-1b20-413f-a04b-47c23c09c8f3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added cohen's d calculations
</commit_message>
<xml_diff>
--- a/Studies_from_Zhou_NMA.xlsx
+++ b/Studies_from_Zhou_NMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphaelle\Documents\AIM Lab\apples_and_oranges\main_git\apples_oranges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0F7C9A9-2C01-46B0-A1A7-CA19B7BD1BDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9270CF71-C5F5-4421-90BE-5EB3363753CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17560" windowHeight="5810" xr2:uid="{88929F6D-EA7A-425D-B888-A9B6898AEC85}"/>
   </bookViews>
@@ -248,12 +248,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -268,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -276,6 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -594,7 +601,7 @@
   <dimension ref="A1:AK8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6:O7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1213,7 +1220,7 @@
       <c r="O6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P6" s="8">
         <v>24</v>
       </c>
       <c r="Q6">
@@ -1326,7 +1333,7 @@
       <c r="O7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="8">
         <v>24</v>
       </c>
       <c r="Q7">
@@ -1699,15 +1706,15 @@
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18ECBF79-BB4A-488F-B9C8-31A27F727F35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="bdfa4711-3526-46a9-86fc-45ee7e9669d1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="0803544b-1b20-413f-a04b-47c23c09c8f3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>